<commit_message>
add printer termal pada transaksi produk
</commit_message>
<xml_diff>
--- a/public/ProdukData/tes impor produk.xlsx
+++ b/public/ProdukData/tes impor produk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaed\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF690A2-47B6-46C9-A9A8-F83EC86A126A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E6B67B-5900-469F-97DF-F976F21EF9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -52,19 +52,16 @@
     <t>Jaya</t>
   </si>
   <si>
-    <t>Coba 1</t>
-  </si>
-  <si>
-    <t>Coba 2</t>
-  </si>
-  <si>
-    <t>AB-231234</t>
-  </si>
-  <si>
     <t>Tes</t>
   </si>
   <si>
     <t>Agen</t>
+  </si>
+  <si>
+    <t>Coba 3</t>
+  </si>
+  <si>
+    <t>Coba 4</t>
   </si>
 </sst>
 </file>
@@ -432,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
@@ -482,14 +479,9 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>24235234546</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="D2">
         <v>1</v>
       </c>
@@ -511,14 +503,9 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>24235234540</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="D3">
         <v>1</v>
       </c>
@@ -538,7 +525,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>